<commit_message>
DOC - Q&A list update - 인증 관련 사항
</commit_message>
<xml_diff>
--- a/0_DOC/Plasma_Gen_Q&A_list_20180130.xlsx
+++ b/0_DOC/Plasma_Gen_Q&A_list_20180130.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="67">
   <si>
     <t>No</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -303,6 +303,35 @@
   <si>
     <t>추가적으로 동작여부 확인이 필요한 기능에 대한 LED 추가 여부 확인
  - 현재 +5V, +3.3V(MCU On), Plasma On, RS-232 R/Tx 에 대한 상태에 대해서 LED로 정상 동작여부 확인하도록 했으며, 이외에 추가적으로 필요한 부분 확인 바랍니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Straight type or Right angle type?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>GSP Korea
+유재희
+Mobile: +82 10 8648 2090
+Fax     : +82 31 427 8523
+E-mail: jhyoo@gspkorea.co.kr</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>제안 : USB CON 하나로 RS-232 통신과 External 전원 공급 지원</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Certification을 받아야 하는 인증 목록 확인 필요
+Battery를 사용하는 경우 추가 인증이 있을 수 있음</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>보통 국가마다 제품 인증이 필요하며, 아래는 전자제품의 경우 받는 인증들임.
+장비의 경우는 제가 잘 모릅니다.  
+  국내 : KC 인증
+  유럽 : EC 인증
+  미국 : FCC 인증 등등..</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1196,7 +1225,7 @@
   <dimension ref="B1:H31"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1205,7 +1234,7 @@
     <col min="2" max="2" width="6.75" style="1" customWidth="1"/>
     <col min="3" max="3" width="11.125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="9" style="1"/>
-    <col min="6" max="6" width="75.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="70.125" style="1" customWidth="1"/>
     <col min="7" max="7" width="29.625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="57.125" style="20" customWidth="1"/>
     <col min="9" max="16384" width="9" style="1"/>
@@ -1276,7 +1305,9 @@
         <v>9</v>
       </c>
       <c r="G5" s="17"/>
-      <c r="H5" s="23"/>
+      <c r="H5" s="23" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B6" s="5">
@@ -1335,7 +1366,7 @@
       <c r="G8" s="18"/>
       <c r="H8" s="23"/>
     </row>
-    <row r="9" spans="2:8" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:8" ht="82.5" x14ac:dyDescent="0.3">
       <c r="B9" s="5">
         <v>6</v>
       </c>
@@ -1352,7 +1383,9 @@
         <v>25</v>
       </c>
       <c r="G9" s="18"/>
-      <c r="H9" s="23"/>
+      <c r="H9" s="23" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="10" spans="2:8" ht="49.5" x14ac:dyDescent="0.3">
       <c r="B10" s="5">
@@ -1371,7 +1404,9 @@
         <v>29</v>
       </c>
       <c r="G10" s="17"/>
-      <c r="H10" s="23"/>
+      <c r="H10" s="23" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B11" s="5">
@@ -1497,16 +1532,26 @@
       <c r="G16" s="18"/>
       <c r="H16" s="23"/>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:8" ht="99" x14ac:dyDescent="0.3">
       <c r="B17" s="5">
         <v>14</v>
       </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
+      <c r="C17" s="6">
+        <v>43132</v>
+      </c>
+      <c r="D17" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>65</v>
+      </c>
       <c r="G17" s="18"/>
-      <c r="H17" s="23"/>
+      <c r="H17" s="23" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B18" s="5">
@@ -1677,7 +1722,7 @@
   <dimension ref="B1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1687,7 +1732,7 @@
     <col min="3" max="3" width="11.125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="9" style="1"/>
     <col min="6" max="6" width="75.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="44" style="1" customWidth="1"/>
+    <col min="7" max="7" width="38.625" style="1" customWidth="1"/>
     <col min="8" max="8" width="39.125" style="20" customWidth="1"/>
     <col min="9" max="16384" width="9" style="1"/>
   </cols>
@@ -2080,6 +2125,6 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="66" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="68" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>